<commit_message>
general uptade of site
</commit_message>
<xml_diff>
--- a/examples/2024_07_23/graphics.xlsx
+++ b/examples/2024_07_23/graphics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="33540" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,6 +170,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -190,7 +192,44 @@
     <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1063,14 +1102,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:J5" totalsRowShown="0">
   <autoFilter ref="A2:J5"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Concurrency"/>
+    <tableColumn id="1" name="Concurrency" dataDxfId="0"/>
     <tableColumn id="2" name="thread"/>
     <tableColumn id="3" name="processes"/>
     <tableColumn id="4" name="coroutines"/>
-    <tableColumn id="5" name="thread2"/>
+    <tableColumn id="5" name="thread2" dataDxfId="2"/>
     <tableColumn id="6" name="processes2"/>
     <tableColumn id="7" name="coroutines2"/>
-    <tableColumn id="8" name="thread3"/>
+    <tableColumn id="8" name="thread3" dataDxfId="1"/>
     <tableColumn id="9" name="processes3"/>
     <tableColumn id="10" name="coroutines3"/>
   </tableColumns>
@@ -1402,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1435,7 +1474,7 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -1467,7 +1506,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>5</v>
       </c>
       <c r="B3">
@@ -1479,7 +1518,7 @@
       <c r="D3">
         <v>6.23</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>10.73</v>
       </c>
       <c r="F3">
@@ -1488,7 +1527,7 @@
       <c r="G3">
         <v>10.18</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>21.59</v>
       </c>
       <c r="I3">
@@ -1499,7 +1538,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>10</v>
       </c>
       <c r="B4">
@@ -1511,7 +1550,7 @@
       <c r="D4">
         <v>2.8</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>6.38</v>
       </c>
       <c r="F4">
@@ -1520,7 +1559,7 @@
       <c r="G4">
         <v>5.94</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>11.15</v>
       </c>
       <c r="I4">
@@ -1531,7 +1570,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5">
+      <c r="A5" s="6">
         <v>15</v>
       </c>
       <c r="B5">
@@ -1543,7 +1582,7 @@
       <c r="D5">
         <v>2.06</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>3.7</v>
       </c>
       <c r="F5">
@@ -1552,7 +1591,7 @@
       <c r="G5">
         <v>3.87</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>7.85</v>
       </c>
       <c r="I5">

</xml_diff>